<commit_message>
add call function by name
</commit_message>
<xml_diff>
--- a/_Asset/Database/Lines.xlsx
+++ b/_Asset/Database/Lines.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">呀吼! 怎麼了?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Shake</t>
   </si>
   <si>
     <t xml:space="preserve">遙香</t>
@@ -248,10 +251,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,19 +394,19 @@
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>29</v>
@@ -413,8 +416,8 @@
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>30</v>
@@ -424,8 +427,8 @@
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>31</v>
@@ -435,50 +438,57 @@
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="1" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="H14" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="I14" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3"/>
@@ -499,6 +509,10 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add corresponding char aciton
</commit_message>
<xml_diff>
--- a/_Asset/Database/Lines.xlsx
+++ b/_Asset/Database/Lines.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">阿阿...阿魯大人讓我來找你</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Jump</t>
   </si>
   <si>
     <t xml:space="preserve">找我? 阿魯醬她怎麼了嗎?</t>
@@ -146,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Microsoft JhengHei"/>
@@ -173,6 +176,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -217,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,6 +239,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,10 +263,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -416,10 +428,10 @@
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -427,8 +439,8 @@
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>31</v>
@@ -438,8 +450,8 @@
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>32</v>
@@ -449,50 +461,57 @@
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3"/>
@@ -513,6 +532,10 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
refactor DialogLoader data structure
</commit_message>
<xml_diff>
--- a/_Asset/Database/Lines.xlsx
+++ b/_Asset/Database/Lines.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Result4</t>
   </si>
   <si>
+    <t xml:space="preserve">FinalResults</t>
+  </si>
+  <si>
     <t xml:space="preserve">H1</t>
   </si>
   <si>
@@ -113,6 +116,12 @@
   </si>
   <si>
     <t xml:space="preserve">@Jump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump2</t>
   </si>
   <si>
     <t xml:space="preserve">找我? 阿魯醬她怎麼了嗎?</t>
@@ -263,10 +272,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -312,205 +321,217 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add dialog history panel
</commit_message>
<xml_diff>
--- a/_Asset/Database/Lines.xlsx
+++ b/_Asset/Database/Lines.xlsx
@@ -103,19 +103,19 @@
     <t xml:space="preserve">欸! 是遙香醬</t>
   </si>
   <si>
+    <t xml:space="preserve">@Shake</t>
+  </si>
+  <si>
     <t xml:space="preserve">呀吼! 怎麼了?</t>
   </si>
   <si>
-    <t xml:space="preserve">@Shake</t>
-  </si>
-  <si>
     <t xml:space="preserve">遙香</t>
   </si>
   <si>
+    <t xml:space="preserve">@Jump</t>
+  </si>
+  <si>
     <t xml:space="preserve">阿阿...阿魯大人讓我來找你</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Jump</t>
   </si>
   <si>
     <t xml:space="preserve">找我? 阿魯醬她怎麼了嗎?</t>
@@ -269,7 +269,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -398,7 +398,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -408,8 +408,9 @@
       <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -420,25 +421,26 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="0" t="s">

</xml_diff>